<commit_message>
Aguegamos la lucha en smackdown 74 fatal four way
</commit_message>
<xml_diff>
--- a/Undertaker Matches.xlsx
+++ b/Undertaker Matches.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Taker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCA1654-DC90-4B0B-A700-B9F782AFB41F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AF0614-5EEA-48F5-BAFD-93105A1BA0CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="421">
   <si>
     <t>no.</t>
   </si>
@@ -1284,6 +1284,15 @@
   </si>
   <si>
     <t>The Undertaker Vs. Kane Vs. Steve Austin</t>
+  </si>
+  <si>
+    <t>09.01.2001</t>
+  </si>
+  <si>
+    <t>Smack Down #74</t>
+  </si>
+  <si>
+    <t>The Undertaker Vs. Kane Vs. Rikishi Vs. The Rock</t>
   </si>
 </sst>
 </file>
@@ -1375,7 +1384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1408,6 +1417,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1691,7 +1701,7 @@
   <dimension ref="A1:E369"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A176" workbookViewId="0">
-      <selection activeCell="C196" sqref="C196"/>
+      <selection activeCell="D197" sqref="D197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4447,8 +4457,14 @@
       <c r="A195" s="6">
         <v>194</v>
       </c>
-      <c r="C195" s="1">
-        <v>2001</v>
+      <c r="B195" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D195" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="196" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
@@ -4460,6 +4476,7 @@
       <c r="A197" s="6">
         <v>196</v>
       </c>
+      <c r="D197" s="16"/>
     </row>
     <row r="198" spans="1:4" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A198" s="6">

</xml_diff>

<commit_message>
RR93, RAW, WM9 - 35min
</commit_message>
<xml_diff>
--- a/Undertaker Matches.xlsx
+++ b/Undertaker Matches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\descargas\Taker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F33FF4D-555C-40E7-AF66-70F988851943}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E87E945-D7E4-439C-AB4C-671727FD2B9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="1249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1619" uniqueCount="1250">
   <si>
     <t>match</t>
   </si>
@@ -3787,6 +3787,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>min 35</t>
   </si>
 </sst>
 </file>
@@ -3834,7 +3837,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3850,6 +3853,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3881,7 +3890,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3953,6 +3962,9 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4236,8 +4248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F517"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -4246,7 +4258,7 @@
     <col min="2" max="2" width="39" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" style="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="159.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="84" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4418,20 +4430,20 @@
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="7">
+    <row r="12" spans="1:6" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="15">
         <v>11</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
@@ -4446,7 +4458,7 @@
       <c r="D13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
@@ -4461,7 +4473,9 @@
       <c r="D14" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="28" t="s">
+        <v>1249</v>
+      </c>
       <c r="F14" t="s">
         <v>1181</v>
       </c>

</xml_diff>